<commit_message>
testDir and testMatch added
</commit_message>
<xml_diff>
--- a/configinfo.xlsx
+++ b/configinfo.xlsx
@@ -16,28 +16,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t xml:space="preserve">No fields are mandatory, if you don't provide it will search whole project root for .spec or .test by default. But after whole search if any .only is found it will switch its default setting that was searching for .spec or .test and running all to just searching for .only specified test and running.</t>
+  </si>
   <si>
     <t>Property</t>
   </si>
   <si>
-    <t xml:space="preserve">Mandatory Y/N</t>
-  </si>
-  <si>
     <t>Path</t>
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>testDir</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searches for by default in specified and directories inside that recursively</t>
+  </si>
+  <si>
+    <t>testMatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">specify regex or string pattern to search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color indexed="2"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
@@ -62,8 +84,9 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -569,26 +592,55 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="15.421875"/>
-    <col customWidth="1" min="3" max="3" width="11.8515625"/>
-    <col customWidth="1" min="4" max="4" width="110.421875"/>
+    <col customWidth="1" min="1" max="1" width="15.421875"/>
+    <col customWidth="1" min="2" max="2" width="11.8515625"/>
+    <col customWidth="1" min="3" max="3" width="110.421875"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25">
-      <c r="A1" t="s">
+    <row r="1" ht="49" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>

</xml_diff>

<commit_message>
screenshot and updated notes
</commit_message>
<xml_diff>
--- a/configinfo.xlsx
+++ b/configinfo.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t xml:space="preserve">No fields are mandatory, if you don't provide it will search whole project root for .spec or .test by default. 
 But after whole search if any .only is found it will switch its default setting that was searching for .spec or .test and running all to just searching for .only specified test and running.</t>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">outputDir</t>
   </si>
   <si>
-    <t xml:space="preserve">outputDir property is a configuration setting that determines where test artifacts are saved during and after a test run. Related to-Failed test screenshots, Video recordings, Trace files (.zip) and attached attributes</t>
+    <t xml:space="preserve">outputDir property is a configuration setting that determines where test artifacts are saved during and after a test run. Related to-all values supported in screenshot prop in use playwright config, Video recordings, Trace files (.zip) and attached attributes</t>
   </si>
   <si>
     <t xml:space="preserve">globalSetup</t>
@@ -174,6 +174,21 @@
   </si>
   <si>
     <t xml:space="preserve">tell browser name in which test executes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">screenshot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">property with allowed values:'off' | 'on' | 'only-on-failure' | 'on-first-failure'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on: Takes a screenshot for every single test (high storage usage).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only-on-failure: The most popular choice; it only saves a screenshot if the test fails.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">on-first-retry: Only takes it if the test failed once and is being retried.</t>
   </si>
 </sst>
 </file>
@@ -183,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,18 +257,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -347,16 +350,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -551,7 +554,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -763,16 +766,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="75.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="75.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,53 +789,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="http://localhost:3000"/>
+    <hyperlink ref="C3" r:id="rId1" display="baseURL is use to set base url like http://localhost:3000 and in your testcase you can add just path"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
name property in project object
</commit_message>
<xml_diff>
--- a/configinfo.xlsx
+++ b/configinfo.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="root level" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="use level" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="project level" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="59">
   <si>
     <t xml:space="preserve">No fields are mandatory, if you don't provide it will search whole project root for .spec or .test by default. 
 But after whole search if any .only is found it will switch its default setting that was searching for .spec or .test and running all to just searching for .only specified test and running.</t>
@@ -211,6 +212,15 @@
   <si>
     <t xml:space="preserve">storageState is property where we specify json which have stored local storage,auth related,session cookies. And we use same json to call different test and playwright internally add these info while creating context in test/s</t>
   </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unique name given by which we can run config</t>
+  </si>
 </sst>
 </file>
 
@@ -219,7 +229,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,12 +289,6 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -334,7 +338,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,10 +377,6 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -785,8 +785,8 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -902,7 +902,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>52</v>
       </c>
@@ -920,7 +920,7 @@
       <c r="B15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -936,4 +936,54 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="47.93"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating config doc root doc
</commit_message>
<xml_diff>
--- a/configinfo.xlsx
+++ b/configinfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="root level" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t xml:space="preserve">No fields are mandatory, if you don't provide it will search whole project root for .spec or .test by default. 
 But after whole search if any .only is found it will switch its default setting that was searching for .spec or .test and running all to just searching for .only specified test and running.</t>
@@ -148,6 +148,15 @@
   </si>
   <si>
     <t xml:space="preserve">webServer: { url: "http://localhost:9000", timeout: 10000, command: "node ./myserver.js", stdout: "pipe", }  It basically wait for success response then run test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grepInvert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used to ignore scenario by regex provided matches description. If you are using string value directly as value it will not work better to use new RegExp(“string value”)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output ss, video ,trace path</t>
   </si>
   <si>
     <t xml:space="preserve">headless</t>
@@ -273,16 +282,7 @@
     <t xml:space="preserve">used to run scenario by regex provided matches description. If you are using string value directly as value it will not work better to use new RegExp(“string value”)</t>
   </si>
   <si>
-    <t xml:space="preserve">grepInvert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">used to ignore scenario by regex provided matches description. If you are using string value directly as value it will not work better to use new RegExp(“string value”)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Project object use</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output ss, video ,trace path</t>
   </si>
 </sst>
 </file>
@@ -452,12 +452,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -649,10 +649,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -843,6 +843,28 @@
       </c>
       <c r="C17" s="8" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -867,7 +889,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B17:B19 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -889,120 +911,120 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="9" t="s">
-        <v>51</v>
+      <c r="C12" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1026,8 +1048,8 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="B17:B19 A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1049,46 +1071,46 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,54 +1118,54 @@
         <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>66</v>
+      <c r="A9" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>